<commit_message>
small edits to results Excel Sheets
</commit_message>
<xml_diff>
--- a/Results/Picante Tables.xlsx
+++ b/Results/Picante Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{F6C9480E-E46D-411E-B786-ADBAE2B32309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{016C6D9E-D2E0-4A1C-976E-4FE7F27F428E}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F6C9480E-E46D-411E-B786-ADBAE2B32309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46004003-B8B1-4832-8F4F-583B64416E6B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{DFF0E715-C34D-44F2-BAE8-81DAD7E13060}"/>
+    <workbookView xWindow="7850" yWindow="680" windowWidth="11340" windowHeight="9500" firstSheet="1" activeTab="1" xr2:uid="{DFF0E715-C34D-44F2-BAE8-81DAD7E13060}"/>
   </bookViews>
   <sheets>
     <sheet name="Phylogenetic Distance (PD)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Index</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>~0 (7.334e-5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">????? Revisit </t>
   </si>
   <si>
     <t>Sexual Dimorphism - Hue (pc2)</t>
@@ -184,6 +181,12 @@
   </si>
   <si>
     <t>Cooperative Breeding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">look at paper - they may have measured why there isn't strong phylogenetic signal </t>
+  </si>
+  <si>
+    <t>????? Revisit and REDO</t>
   </si>
 </sst>
 </file>
@@ -284,13 +287,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9D2E9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D2E9"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -535,19 +538,25 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -565,6 +574,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -887,7 +900,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,10 +973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14114C9F-AF7B-4376-82A0-47A0FDD6922F}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,7 +984,7 @@
     <col min="1" max="1" width="19.36328125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="4" max="4" width="32" style="35" customWidth="1"/>
+    <col min="4" max="4" width="32" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.4">
@@ -1188,7 +1201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="29" t="s">
         <v>31</v>
       </c>
@@ -1202,35 +1215,40 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="36">
         <v>1</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="30" t="s">
+      <c r="B19" s="36">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="C19" s="36">
+        <v>0.105</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="13">
-        <v>4.1200000000000001E-2</v>
-      </c>
-      <c r="C19" s="13">
-        <v>0.105</v>
-      </c>
-      <c r="D19" s="31"/>
-    </row>
-    <row r="20" spans="1:4" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="B20" s="14">
         <v>0.746</v>
@@ -1239,26 +1257,26 @@
         <v>13</v>
       </c>
       <c r="D20" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="31" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="32" t="s">
-        <v>39</v>
       </c>
       <c r="B21" s="14">
         <v>0.93799999999999994</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="32" t="s">
         <v>40</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="33" t="s">
-        <v>41</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>25</v>
@@ -1270,9 +1288,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="34" t="s">
-        <v>42</v>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
fitDiscrete() - only getting lambda of 0.000
</commit_message>
<xml_diff>
--- a/Results/Picante Tables.xlsx
+++ b/Results/Picante Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{F6C9480E-E46D-411E-B786-ADBAE2B32309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46004003-B8B1-4832-8F4F-583B64416E6B}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{F6C9480E-E46D-411E-B786-ADBAE2B32309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48F5638C-BC85-470A-9FEB-816C94CF9DCC}"/>
   <bookViews>
-    <workbookView xWindow="7850" yWindow="680" windowWidth="11340" windowHeight="9500" firstSheet="1" activeTab="1" xr2:uid="{DFF0E715-C34D-44F2-BAE8-81DAD7E13060}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="1" activeTab="1" xr2:uid="{DFF0E715-C34D-44F2-BAE8-81DAD7E13060}"/>
   </bookViews>
   <sheets>
     <sheet name="Phylogenetic Distance (PD)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Index</t>
   </si>
@@ -117,25 +117,13 @@
     <t>-</t>
   </si>
   <si>
-    <t>not continuous</t>
-  </si>
-  <si>
     <t>Nest Site Low - On or Under the Ground</t>
   </si>
   <si>
     <t>Nest Site High - Above the Ground</t>
   </si>
   <si>
-    <t>Nest Strategy- Enclosed</t>
-  </si>
-  <si>
-    <t>Nest Strategy - Open</t>
-  </si>
-  <si>
     <t>Nest Safety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ordinal?????? Try </t>
   </si>
   <si>
     <t>Sexual Dimorphism- Brightness (pc1)</t>
@@ -183,10 +171,25 @@
     <t>Cooperative Breeding</t>
   </si>
   <si>
-    <t xml:space="preserve">look at paper - they may have measured why there isn't strong phylogenetic signal </t>
-  </si>
-  <si>
-    <t>????? Revisit and REDO</t>
+    <t>continuous</t>
+  </si>
+  <si>
+    <t>discrete</t>
+  </si>
+  <si>
+    <t>numeric ordinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuous - perhaps low because of how we transformed these variables </t>
+  </si>
+  <si>
+    <t>Nest Strategy- Enclosed/Open</t>
+  </si>
+  <si>
+    <t>discrete - using model = "ER" (equal rates)</t>
+  </si>
+  <si>
+    <t>no p value given by fitDiscrete()</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -442,11 +445,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -514,9 +530,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -526,9 +539,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -550,13 +560,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -565,6 +599,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEAD1DC"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFFCCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -574,10 +615,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -973,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14114C9F-AF7B-4376-82A0-47A0FDD6922F}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +1021,7 @@
     <col min="1" max="1" width="19.36328125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="4" max="4" width="32" style="34" customWidth="1"/>
+    <col min="4" max="4" width="32" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.4">
@@ -1011,7 +1048,9 @@
       <c r="C2" s="11">
         <v>0</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
@@ -1023,7 +1062,9 @@
       <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
@@ -1032,10 +1073,12 @@
       <c r="B4" s="10">
         <v>0.93600000000000005</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="19" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
@@ -1044,10 +1087,10 @@
       <c r="B5" s="13">
         <v>0.84499999999999997</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1103,7 +1146,9 @@
       <c r="C9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="20" t="s">
@@ -1115,7 +1160,7 @@
       <c r="C10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1129,10 +1174,12 @@
       <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1141,142 +1188,139 @@
       <c r="C12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="28" t="s">
+      <c r="B13" s="33">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="33">
+        <v>0</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="33">
+        <v>0</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="19">
+        <v>0.876</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="34">
+        <v>1</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="34">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="C18" s="38">
+        <v>0.105</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="24">
+        <v>0.746</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="14">
-        <v>0.876</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="36">
-        <v>1</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="36">
-        <v>4.1200000000000001E-2</v>
-      </c>
-      <c r="C19" s="36">
-        <v>0.105</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="14">
-        <v>0.746</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="D21" s="42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="31" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="14">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="32" t="s">
-        <v>40</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>25</v>
@@ -1284,22 +1328,8 @@
       <c r="C22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>26</v>
+      <c r="D22" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>